<commit_message>
docs: Style compute instance performance comparison sheet.
</commit_message>
<xml_diff>
--- a/projects/03_image-classification-aws-sagemaker/doc/compute-instance-performance-comparison.xlsx
+++ b/projects/03_image-classification-aws-sagemaker/doc/compute-instance-performance-comparison.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -31,13 +31,13 @@
     <t xml:space="preserve">cost/hour</t>
   </si>
   <si>
-    <t xml:space="preserve">Epoch training time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epoch testing time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">setup time</t>
+    <t xml:space="preserve">Epoch training time(sec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch testing time(sec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">setup time(sec)</t>
   </si>
   <si>
     <t xml:space="preserve">training cost/epoch</t>
@@ -82,6 +82,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -181,19 +182,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -212,14 +214,13 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -239,17 +240,17 @@
       <c r="E2" s="1" t="n">
         <v>156.01</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="F2" s="0" t="n">
         <f aca="false">B2-(D2+E2)</f>
         <v>175.62</v>
       </c>
-      <c r="H2" s="1" t="n">
-        <f aca="false">D2*C2/3600</f>
-        <v>0.0526562638888889</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <f aca="false">B2*C2/3600</f>
-        <v>0.06325</v>
+      <c r="G2" s="1" t="n">
+        <f aca="false">ROUND(D2*C2/3600,3)</f>
+        <v>0.053</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">ROUND(B2*C2/3600,3)</f>
+        <v>0.063</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -268,17 +269,17 @@
       <c r="E3" s="1" t="n">
         <v>92.23</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="F3" s="0" t="n">
         <f aca="false">B3-(D3+E3)</f>
         <v>177.58</v>
       </c>
-      <c r="H3" s="1" t="n">
-        <f aca="false">D3*C3/3600</f>
-        <v>0.0571288055555556</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <f aca="false">B3*C3/3600</f>
-        <v>0.0743666666666667</v>
+      <c r="G3" s="1" t="n">
+        <f aca="false">ROUND(D3*C3/3600,3)</f>
+        <v>0.057</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">ROUND(B3*C3/3600,3)</f>
+        <v>0.074</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -297,17 +298,17 @@
       <c r="E4" s="1" t="n">
         <v>16.18</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="F4" s="0" t="n">
         <f aca="false">B4-(D4+E4)</f>
         <v>421.3</v>
       </c>
-      <c r="H4" s="1" t="n">
-        <f aca="false">D4*C4/3600</f>
-        <v>0.0511</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <f aca="false">B4*C4/3600</f>
-        <v>0.1878125</v>
+      <c r="G4" s="1" t="n">
+        <f aca="false">ROUND(D4*C4/3600,3)</f>
+        <v>0.051</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">ROUND(B4*C4/3600,3)</f>
+        <v>0.188</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -326,17 +327,17 @@
       <c r="E5" s="1" t="n">
         <v>46.23</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="F5" s="0" t="n">
         <f aca="false">B5-(D5+E5)</f>
         <v>155.39</v>
       </c>
-      <c r="H5" s="1" t="n">
-        <f aca="false">D5*C5/3600</f>
-        <v>0.0861506555555556</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <f aca="false">B5*C5/3600</f>
-        <v>0.137787777777778</v>
+      <c r="G5" s="1" t="n">
+        <f aca="false">ROUND(D5*C5/3600,3)</f>
+        <v>0.086</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">ROUND(B5*C5/3600,3)</f>
+        <v>0.138</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -355,17 +356,17 @@
       <c r="E6" s="1" t="n">
         <v>52.32</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="F6" s="0" t="n">
         <f aca="false">B6-(D6+E6)</f>
         <v>197.13</v>
       </c>
-      <c r="H6" s="1" t="n">
-        <f aca="false">D6*C6/3600</f>
-        <v>0.105726458333333</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <f aca="false">B6*C6/3600</f>
-        <v>0.1719</v>
+      <c r="G6" s="1" t="n">
+        <f aca="false">ROUND(D6*C6/3600,3)</f>
+        <v>0.106</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">ROUND(B6*C6/3600,3)</f>
+        <v>0.172</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,17 +385,17 @@
       <c r="E7" s="1" t="n">
         <v>60.69</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="F7" s="0" t="n">
         <f aca="false">B7-(D7+E7)</f>
         <v>162.91</v>
       </c>
-      <c r="H7" s="1" t="n">
-        <f aca="false">D7*C7/3600</f>
-        <v>0.066384</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <f aca="false">B7*C7/3600</f>
-        <v>0.0950172222222222</v>
+      <c r="G7" s="1" t="n">
+        <f aca="false">ROUND(D7*C7/3600,3)</f>
+        <v>0.066</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <f aca="false">ROUND(B7*C7/3600,3)</f>
+        <v>0.095</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,17 +414,17 @@
       <c r="E8" s="1" t="n">
         <v>9.67</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="F8" s="0" t="n">
         <f aca="false">B8-(D8+E8)</f>
         <v>351.91</v>
       </c>
-      <c r="H8" s="1" t="n">
-        <f aca="false">D8*C8/3600</f>
-        <v>0.1513455</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <f aca="false">B8*C8/3600</f>
-        <v>0.642491666666667</v>
+      <c r="G8" s="1" t="n">
+        <f aca="false">ROUND(D8*C8/3600,3)</f>
+        <v>0.151</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">ROUND(B8*C8/3600,3)</f>
+        <v>0.642</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -442,17 +443,17 @@
       <c r="E9" s="1" t="n">
         <v>11.17</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="F9" s="0" t="n">
         <f aca="false">B9-(D9+E9)</f>
         <v>375.24</v>
       </c>
-      <c r="H9" s="1" t="n">
-        <f aca="false">D9*C9/3600</f>
-        <v>0.115376875</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <f aca="false">B9*C9/3600</f>
-        <v>0.5259375</v>
+      <c r="G9" s="1" t="n">
+        <f aca="false">ROUND(D9*C9/3600,3)</f>
+        <v>0.115</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <f aca="false">ROUND(B9*C9/3600,3)</f>
+        <v>0.526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>